<commit_message>
Added a iterator check to EmployeeInputRecord so that it will not cast a "NoSuchElementException" when it is out of rows.
</commit_message>
<xml_diff>
--- a/code/job/src/test/resources/test_data.xlsx
+++ b/code/job/src/test/resources/test_data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Navn</t>
   </si>
@@ -32,45 +32,37 @@
     <t>Navn 1</t>
   </si>
   <si>
-    <t>navn1@accenture.com</t>
-  </si>
-  <si>
-    <t>AD/navn1</t>
+    <t>navn1.etternavn@accenture.com</t>
+  </si>
+  <si>
+    <t>navn1.etternavn</t>
   </si>
   <si>
     <t>Navn 2</t>
   </si>
   <si>
-    <t>navn2@accenture.com</t>
-  </si>
-  <si>
-    <t>AD/navn2</t>
+    <t>navn2.etternavn@accenture.com</t>
   </si>
   <si>
     <t>Navn 3</t>
   </si>
   <si>
-    <t>navn3@accenture.com</t>
-  </si>
-  <si>
-    <t>AD/navn3</t>
+    <t>navn3.etternavn@accenture.com</t>
   </si>
   <si>
     <t>Navn 4</t>
   </si>
   <si>
-    <t>navn4@accenture.com</t>
-  </si>
-  <si>
-    <t>AD/navn4</t>
+    <t>navn4.etternavn@accenture.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
+    <numFmt formatCode="General" numFmtId="165"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -151,7 +143,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -160,7 +152,11 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="165" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -181,10 +177,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D5" activeCellId="0" pane="topLeft" sqref="D5"/>
+      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -203,7 +199,7 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -217,7 +213,7 @@
       <c r="B2" s="0" t="n">
         <v>251244</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="0" t="s">
@@ -231,47 +227,51 @@
       <c r="B3" s="0" t="n">
         <v>511225</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>543312</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>11</v>
+      <c r="C4" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>532122</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>14</v>
+      <c r="C5" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
+        <v>6</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="6"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="7"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="8"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="9"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="navn1@accenture.com" ref="C2" r:id="rId1"/>
-    <hyperlink display="navn2@accenture.com" ref="C3" r:id="rId2"/>
-    <hyperlink display="navn3@accenture.com" ref="C4" r:id="rId3"/>
-    <hyperlink display="navn4@accenture.com" ref="C5" r:id="rId4"/>
+    <hyperlink display="navn1.etternavn@accenture.com" ref="C2" r:id="rId1"/>
+    <hyperlink display="navn2.etternavn@accenture.com" ref="C3" r:id="rId2"/>
+    <hyperlink display="navn3.etternavn@accenture.com" ref="C4" r:id="rId3"/>
+    <hyperlink display="navn4.etternavn@accenture.com" ref="C5" r:id="rId4"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>